<commit_message>
Added nmrshiftdb calculation of carbon chemical shifts so that we can overlay nodes onto correct carbon on image. Added a new dialog to ask user which method of overlay they want. Fixed bug on dragging so zoom now works if clicked on toolbar Fixed bug when dragging node outside of plot window which resulted in an error for matplotlib trying to convert None values to floats when updating screen. If x or y coordinates are None then drag call back return without updating molecule plot.
</commit_message>
<xml_diff>
--- a/exampleProblems/nowick/nowick.xlsx
+++ b/exampleProblems/nowick/nowick.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/nowick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{20C417E0-FAD9-0345-8769-237C446526CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E124B865-6398-4035-8274-159D46C6CE54}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{20C417E0-FAD9-0345-8769-237C446526CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E23E4F9-B81A-44B9-9434-F31876765C2A}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="990" windowWidth="20295" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7620" yWindow="1335" windowWidth="20295" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>smiles</t>
+  </si>
+  <si>
+    <t>CC(C)C1COC12CCN(C)C2=O</t>
   </si>
 </sst>
 </file>
@@ -704,6 +707,7 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -720,6 +724,9 @@
       </c>
       <c r="B2" t="s">
         <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4099,21 +4106,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100155B07917A39914F9664B9093559A33D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbeff89c08116489e82681c46e7ae15d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6191221-55a2-427d-afce-6bfcc029a585" xmlns:ns4="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a905948312a67a3512ded1d64743b24d" ns3:_="" ns4:_="">
     <xsd:import namespace="f6191221-55a2-427d-afce-6bfcc029a585"/>
@@ -4330,32 +4322,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCEF473A-5319-4ED2-888F-44217AC86176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4372,4 +4354,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>